<commit_message>
5 tests passed, and main working
</commit_message>
<xml_diff>
--- a/tests/test_data.xlsx
+++ b/tests/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RPrince\Documents\python-git-class\london_underground\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23861C2D-163F-492F-8509-809A3F6072A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8691050F-98E8-4E21-B8FC-305B3548A3B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -443,7 +443,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,7 +505,7 @@
         <v>10</v>
       </c>
       <c r="F2">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G2">
         <v>20</v>
@@ -514,7 +514,7 @@
         <v>20</v>
       </c>
       <c r="I2">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>